<commit_message>
added spark motor failure files
</commit_message>
<xml_diff>
--- a/results_analysis/spark-motorFailure/Knn Sparse - Mot Fail - Resumo.xlsx
+++ b/results_analysis/spark-motorFailure/Knn Sparse - Mot Fail - Resumo.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\MLTool_matlab\results_analysis\knn-sparse_motor_failure\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\spark-motorFailure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{808E0A89-A716-4B8B-8D1E-232F30FFBD59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA7D0F8-0652-4A03-9C5D-6587140D13B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="15600" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -36,12 +36,6 @@
     <t>Design Method</t>
   </si>
   <si>
-    <t>NN x KNN</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Coherence</t>
   </si>
   <si>
@@ -76,6 +70,12 @@
   </si>
   <si>
     <t>kmod</t>
+  </si>
+  <si>
+    <t>1-NN x K-NN</t>
+  </si>
+  <si>
+    <t>k</t>
   </si>
 </sst>
 </file>
@@ -754,26 +754,20 @@
   <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.42578125" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" customWidth="1"/>
-    <col min="7" max="7" width="13.42578125" customWidth="1"/>
-    <col min="9" max="9" width="9.7109375" customWidth="1"/>
-    <col min="10" max="10" width="10.42578125" customWidth="1"/>
-    <col min="11" max="11" width="9.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.21875" style="1" customWidth="1"/>
+    <col min="4" max="11" width="17.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A1" s="28" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -786,8 +780,8 @@
       <c r="J1" s="28"/>
       <c r="K1" s="28"/>
     </row>
-    <row r="2" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
@@ -795,34 +789,34 @@
         <v>2</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="D3" s="25" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="26" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="26" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" s="26" t="s">
+      <c r="H3" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="I3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="J3" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="K3" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="K3" s="27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -857,10 +851,10 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="4"/>
       <c r="C5" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D5" s="14">
         <v>63</v>
@@ -887,7 +881,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
       <c r="B6" s="1">
         <v>2</v>
@@ -920,11 +914,11 @@
         <v>83</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D7" s="16">
         <v>33</v>
@@ -951,9 +945,9 @@
         <v>87</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B8" s="3">
         <v>1</v>
@@ -986,10 +980,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A9" s="4"/>
       <c r="C9" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D9" s="14">
         <v>79</v>
@@ -1016,7 +1010,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A10" s="4"/>
       <c r="B10" s="1">
         <v>2</v>
@@ -1049,11 +1043,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D11" s="16">
         <v>78</v>
@@ -1080,9 +1074,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B12" s="3">
         <v>1</v>
@@ -1115,10 +1109,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="C13" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D13" s="14">
         <v>90</v>
@@ -1145,7 +1139,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A14" s="4"/>
       <c r="B14" s="1">
         <v>2</v>
@@ -1178,11 +1172,11 @@
         <v>51</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="5"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D15" s="16">
         <v>48</v>
@@ -1209,9 +1203,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B16" s="1">
         <v>1</v>
@@ -1244,10 +1238,10 @@
         <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A17" s="4"/>
       <c r="C17" s="1" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D17" s="14">
         <v>91</v>
@@ -1274,7 +1268,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A18" s="4"/>
       <c r="B18" s="1">
         <v>2</v>
@@ -1307,11 +1301,11 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="5"/>
       <c r="B19" s="6"/>
       <c r="C19" s="6" t="s">
-        <v>4</v>
+        <v>16</v>
       </c>
       <c r="D19" s="16">
         <v>71</v>

</xml_diff>

<commit_message>
organized boxplot doc file of spark motor fail results
</commit_message>
<xml_diff>
--- a/results_analysis/spark-motorFailure/Knn Sparse - Mot Fail - Resumo.xlsx
+++ b/results_analysis/spark-motorFailure/Knn Sparse - Mot Fail - Resumo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Documents\mltool_matlab\results_analysis\spark-motorFailure\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA7D0F8-0652-4A03-9C5D-6587140D13B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAA6D54B-6046-48B2-A77C-D1034A57E071}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
   <si>
     <t>Sparsiciation Method</t>
   </si>
@@ -77,6 +77,12 @@
   <si>
     <t>k</t>
   </si>
+  <si>
+    <t>MEAN</t>
+  </si>
+  <si>
+    <t>MEDIAN</t>
+  </si>
 </sst>
 </file>
 
@@ -385,7 +391,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -453,12 +459,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -466,6 +466,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -751,10 +763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -766,19 +778,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="30" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="B1" s="30"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="30"/>
+      <c r="K1" s="30"/>
     </row>
     <row r="2" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -791,28 +803,28 @@
       <c r="C3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="26" t="s">
+      <c r="F3" s="24" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="24" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="24" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="27" t="s">
+      <c r="K3" s="25" t="s">
         <v>14</v>
       </c>
     </row>
@@ -826,7 +838,7 @@
       <c r="C4" s="3">
         <v>1</v>
       </c>
-      <c r="D4" s="23">
+      <c r="D4" s="29">
         <v>70</v>
       </c>
       <c r="E4" s="10">
@@ -847,7 +859,7 @@
       <c r="J4" s="10">
         <v>63</v>
       </c>
-      <c r="K4" s="24">
+      <c r="K4" s="26">
         <v>80</v>
       </c>
     </row>
@@ -877,7 +889,7 @@
       <c r="J5" s="8">
         <v>85</v>
       </c>
-      <c r="K5" s="15">
+      <c r="K5" s="21">
         <v>83</v>
       </c>
     </row>
@@ -910,7 +922,7 @@
       <c r="J6" s="8">
         <v>72</v>
       </c>
-      <c r="K6" s="15">
+      <c r="K6" s="21">
         <v>83</v>
       </c>
     </row>
@@ -941,7 +953,7 @@
       <c r="J7" s="17">
         <v>68</v>
       </c>
-      <c r="K7" s="19">
+      <c r="K7" s="22">
         <v>87</v>
       </c>
     </row>
@@ -961,7 +973,7 @@
       <c r="E8" s="12">
         <v>75</v>
       </c>
-      <c r="F8" s="13">
+      <c r="F8" s="12">
         <v>87</v>
       </c>
       <c r="G8" s="13">
@@ -1330,6 +1342,855 @@
       </c>
       <c r="K19" s="22">
         <v>83</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" s="27">
+        <v>0.69605263157894703</v>
+      </c>
+      <c r="E21" s="27">
+        <v>0.73223684210526296</v>
+      </c>
+      <c r="F21" s="27">
+        <v>0.71118421052631597</v>
+      </c>
+      <c r="G21" s="27">
+        <v>0.85065789473684195</v>
+      </c>
+      <c r="H21" s="27">
+        <v>0.87565789473684197</v>
+      </c>
+      <c r="I21" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="27">
+        <v>0.61184210526315796</v>
+      </c>
+      <c r="K21" s="27">
+        <v>0.78092105263157896</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="B22" s="28"/>
+      <c r="D22" s="27">
+        <v>0.63289473684210495</v>
+      </c>
+      <c r="E22" s="27">
+        <v>0.80197368421052595</v>
+      </c>
+      <c r="F22" s="27">
+        <v>0.70657894736842097</v>
+      </c>
+      <c r="G22" s="27">
+        <v>0.84934210526315801</v>
+      </c>
+      <c r="H22" s="27">
+        <v>0.86315789473684201</v>
+      </c>
+      <c r="I22" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J22" s="27">
+        <v>0.64407894736842097</v>
+      </c>
+      <c r="K22" s="27">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D23" s="27">
+        <v>0.70855263157894699</v>
+      </c>
+      <c r="E23" s="27">
+        <v>0.78881578947368403</v>
+      </c>
+      <c r="F23" s="27">
+        <v>0.78355263157894695</v>
+      </c>
+      <c r="G23" s="27">
+        <v>0.83223684210526305</v>
+      </c>
+      <c r="H23" s="27">
+        <v>0.861184210526316</v>
+      </c>
+      <c r="I23" s="27">
+        <v>0.46842105263157902</v>
+      </c>
+      <c r="J23" s="27">
+        <v>0.67960526315789505</v>
+      </c>
+      <c r="K23" s="27">
+        <v>0.81118421052631595</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D24" s="27">
+        <v>0.68947368421052602</v>
+      </c>
+      <c r="E24" s="27">
+        <v>0.80394736842105297</v>
+      </c>
+      <c r="F24" s="27">
+        <v>0.74473684210526303</v>
+      </c>
+      <c r="G24" s="27">
+        <v>0.88815789473684204</v>
+      </c>
+      <c r="H24" s="27">
+        <v>0.79671052631578898</v>
+      </c>
+      <c r="I24" s="27">
+        <v>0.55723684210526303</v>
+      </c>
+      <c r="J24" s="27">
+        <v>0.65526315789473699</v>
+      </c>
+      <c r="K24" s="27">
+        <v>0.85263157894736796</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D25" s="27">
+        <v>0.77039473684210502</v>
+      </c>
+      <c r="E25" s="27">
+        <v>0.731578947368421</v>
+      </c>
+      <c r="F25" s="27">
+        <v>0.84342105263157896</v>
+      </c>
+      <c r="G25" s="27">
+        <v>0.86447368421052595</v>
+      </c>
+      <c r="H25" s="27">
+        <v>0.90723684210526301</v>
+      </c>
+      <c r="I25" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J25" s="27">
+        <v>0.79605263157894701</v>
+      </c>
+      <c r="K25" s="27">
+        <v>0.89144736842105299</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D26" s="27">
+        <v>0.75789473684210495</v>
+      </c>
+      <c r="E26" s="27">
+        <v>0.84276315789473699</v>
+      </c>
+      <c r="F26" s="27">
+        <v>0.72368421052631604</v>
+      </c>
+      <c r="G26" s="27">
+        <v>0.87763157894736898</v>
+      </c>
+      <c r="H26" s="27">
+        <v>0.955921052631579</v>
+      </c>
+      <c r="I26" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J26" s="27">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="K26" s="27">
+        <v>0.893421052631579</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D27" s="27">
+        <v>0.82302631578947405</v>
+      </c>
+      <c r="E27" s="27">
+        <v>0.75</v>
+      </c>
+      <c r="F27" s="27">
+        <v>0.78355263157894695</v>
+      </c>
+      <c r="G27" s="27">
+        <v>0.84276315789473699</v>
+      </c>
+      <c r="H27" s="27">
+        <v>0.88947368421052597</v>
+      </c>
+      <c r="I27" s="27">
+        <v>0.54934210526315796</v>
+      </c>
+      <c r="J27" s="27">
+        <v>0.74671052631579005</v>
+      </c>
+      <c r="K27" s="27">
+        <v>0.79802631578947403</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D28" s="27">
+        <v>0.76249999999999996</v>
+      </c>
+      <c r="E28" s="27">
+        <v>0.82960526315789496</v>
+      </c>
+      <c r="F28" s="27">
+        <v>0.73421052631578998</v>
+      </c>
+      <c r="G28" s="27">
+        <v>0.85131578947368403</v>
+      </c>
+      <c r="H28" s="27">
+        <v>0.91710526315789498</v>
+      </c>
+      <c r="I28" s="27">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="J28" s="27">
+        <v>0.74934210526315803</v>
+      </c>
+      <c r="K28" s="27">
+        <v>0.86315789473684201</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D29" s="27">
+        <v>0.90460526315789502</v>
+      </c>
+      <c r="E29" s="27">
+        <v>0.78157894736842104</v>
+      </c>
+      <c r="F29" s="27">
+        <v>0.82763157894736905</v>
+      </c>
+      <c r="G29" s="27">
+        <v>0.85328947368421104</v>
+      </c>
+      <c r="H29" s="27">
+        <v>0.83750000000000002</v>
+      </c>
+      <c r="I29" s="27">
+        <v>0.89539473684210502</v>
+      </c>
+      <c r="J29" s="27">
+        <v>0.817105263157895</v>
+      </c>
+      <c r="K29" s="27">
+        <v>0.86052631578947403</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D30" s="27">
+        <v>0.86776315789473701</v>
+      </c>
+      <c r="E30" s="27">
+        <v>0.88486842105263197</v>
+      </c>
+      <c r="F30" s="27">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="G30" s="27">
+        <v>0.94605263157894803</v>
+      </c>
+      <c r="H30" s="27">
+        <v>0.90394736842105206</v>
+      </c>
+      <c r="I30" s="27">
+        <v>0.89736842105263204</v>
+      </c>
+      <c r="J30" s="27">
+        <v>0.75592105263157905</v>
+      </c>
+      <c r="K30" s="27">
+        <v>0.87302631578947398</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D31" s="27">
+        <v>0.54210526315789498</v>
+      </c>
+      <c r="E31" s="27">
+        <v>0.52171052631578996</v>
+      </c>
+      <c r="F31" s="27">
+        <v>0.518421052631579</v>
+      </c>
+      <c r="G31" s="27">
+        <v>0.54144736842105301</v>
+      </c>
+      <c r="H31" s="27">
+        <v>0.50657894736842102</v>
+      </c>
+      <c r="I31" s="27">
+        <v>0.54539473684210504</v>
+      </c>
+      <c r="J31" s="27">
+        <v>0.51644736842105299</v>
+      </c>
+      <c r="K31" s="27">
+        <v>0.51776315789473704</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D32" s="27">
+        <v>0.54276315789473695</v>
+      </c>
+      <c r="E32" s="27">
+        <v>0.49605263157894702</v>
+      </c>
+      <c r="F32" s="27">
+        <v>0.59934210526315801</v>
+      </c>
+      <c r="G32" s="27">
+        <v>0.51644736842105299</v>
+      </c>
+      <c r="H32" s="27">
+        <v>0.54671052631578998</v>
+      </c>
+      <c r="I32" s="27">
+        <v>0.53157894736842104</v>
+      </c>
+      <c r="J32" s="27">
+        <v>0.55592105263157898</v>
+      </c>
+      <c r="K32" s="27">
+        <v>0.50986842105263197</v>
+      </c>
+    </row>
+    <row r="33" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D33" s="27">
+        <v>0.91644736842105301</v>
+      </c>
+      <c r="E33" s="27">
+        <v>0.92105263157894801</v>
+      </c>
+      <c r="F33" s="27">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="G33" s="27">
+        <v>0.91973684210526296</v>
+      </c>
+      <c r="H33" s="27">
+        <v>0.93157894736842095</v>
+      </c>
+      <c r="I33" s="27">
+        <v>0.548684210526316</v>
+      </c>
+      <c r="J33" s="27">
+        <v>0.77105263157894699</v>
+      </c>
+      <c r="K33" s="27">
+        <v>0.92105263157894801</v>
+      </c>
+    </row>
+    <row r="34" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D34" s="27">
+        <v>0.91052631578947396</v>
+      </c>
+      <c r="E34" s="27">
+        <v>0.90526315789473699</v>
+      </c>
+      <c r="F34" s="27">
+        <v>0.76578947368421102</v>
+      </c>
+      <c r="G34" s="27">
+        <v>0.92171052631578898</v>
+      </c>
+      <c r="H34" s="27">
+        <v>0.90855263157894695</v>
+      </c>
+      <c r="I34" s="27">
+        <v>0.50592105263157905</v>
+      </c>
+      <c r="J34" s="27">
+        <v>0.67434210526315796</v>
+      </c>
+      <c r="K34" s="27">
+        <v>0.88815789473684204</v>
+      </c>
+    </row>
+    <row r="35" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D35" s="27">
+        <v>0.69868421052631602</v>
+      </c>
+      <c r="E35" s="27">
+        <v>0.69342105263157905</v>
+      </c>
+      <c r="F35" s="27">
+        <v>0.75526315789473697</v>
+      </c>
+      <c r="G35" s="27">
+        <v>0.76315789473684204</v>
+      </c>
+      <c r="H35" s="27">
+        <v>0.80460526315789505</v>
+      </c>
+      <c r="I35" s="27">
+        <v>0.56052631578947398</v>
+      </c>
+      <c r="J35" s="27">
+        <v>0.69473684210526299</v>
+      </c>
+      <c r="K35" s="27">
+        <v>0.76644736842105299</v>
+      </c>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D36" s="27">
+        <v>0.67500000000000004</v>
+      </c>
+      <c r="E36" s="27">
+        <v>0.72499999999999998</v>
+      </c>
+      <c r="F36" s="27">
+        <v>0.73750000000000004</v>
+      </c>
+      <c r="G36" s="27">
+        <v>0.87631578947368405</v>
+      </c>
+      <c r="H36" s="27">
+        <v>0.88486842105263197</v>
+      </c>
+      <c r="I36" s="27">
+        <v>0.54605263157894701</v>
+      </c>
+      <c r="J36" s="27">
+        <v>0.63421052631579</v>
+      </c>
+      <c r="K36" s="27">
+        <v>0.81973684210526299</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="B38" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D38" s="27">
+        <v>0.69407894736842102</v>
+      </c>
+      <c r="E38" s="27">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="F38" s="27">
+        <v>0.69736842105263197</v>
+      </c>
+      <c r="G38" s="27">
+        <v>0.89144736842105299</v>
+      </c>
+      <c r="H38" s="27">
+        <v>0.90131578947368396</v>
+      </c>
+      <c r="I38" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J38" s="27">
+        <v>0.61184210526315796</v>
+      </c>
+      <c r="K38" s="27">
+        <v>0.74671052631579005</v>
+      </c>
+    </row>
+    <row r="39" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D39" s="27">
+        <v>0.64144736842105299</v>
+      </c>
+      <c r="E39" s="27">
+        <v>0.8125</v>
+      </c>
+      <c r="F39" s="27">
+        <v>0.68092105263157898</v>
+      </c>
+      <c r="G39" s="27">
+        <v>0.90789473684210498</v>
+      </c>
+      <c r="H39" s="27">
+        <v>0.90131578947368396</v>
+      </c>
+      <c r="I39" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J39" s="27">
+        <v>0.65789473684210498</v>
+      </c>
+      <c r="K39" s="27">
+        <v>0.86184210526315796</v>
+      </c>
+    </row>
+    <row r="40" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D40" s="27">
+        <v>0.71052631578947401</v>
+      </c>
+      <c r="E40" s="27">
+        <v>0.78618421052631604</v>
+      </c>
+      <c r="F40" s="27">
+        <v>0.77302631578947401</v>
+      </c>
+      <c r="G40" s="27">
+        <v>0.87828947368421095</v>
+      </c>
+      <c r="H40" s="27">
+        <v>0.92434210526315796</v>
+      </c>
+      <c r="I40" s="27">
+        <v>0.46052631578947401</v>
+      </c>
+      <c r="J40" s="27">
+        <v>0.67434210526315796</v>
+      </c>
+      <c r="K40" s="27">
+        <v>0.85197368421052599</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D41" s="27">
+        <v>0.68092105263157898</v>
+      </c>
+      <c r="E41" s="27">
+        <v>0.8125</v>
+      </c>
+      <c r="F41" s="27">
+        <v>0.74671052631579005</v>
+      </c>
+      <c r="G41" s="27">
+        <v>0.90789473684210498</v>
+      </c>
+      <c r="H41" s="27">
+        <v>0.85855263157894701</v>
+      </c>
+      <c r="I41" s="27">
+        <v>0.55263157894736803</v>
+      </c>
+      <c r="J41" s="27">
+        <v>0.67105263157894701</v>
+      </c>
+      <c r="K41" s="27">
+        <v>0.91776315789473695</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D42" s="27">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="E42" s="27">
+        <v>0.72697368421052599</v>
+      </c>
+      <c r="F42" s="27">
+        <v>0.86184210526315796</v>
+      </c>
+      <c r="G42" s="27">
+        <v>0.94407894736842102</v>
+      </c>
+      <c r="H42" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="I42" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J42" s="27">
+        <v>0.77960526315789502</v>
+      </c>
+      <c r="K42" s="27">
+        <v>0.93421052631579005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D43" s="27">
+        <v>0.72697368421052599</v>
+      </c>
+      <c r="E43" s="27">
+        <v>0.89144736842105299</v>
+      </c>
+      <c r="F43" s="27">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="G43" s="27">
+        <v>0.9375</v>
+      </c>
+      <c r="H43" s="27">
+        <v>0.96052631578947401</v>
+      </c>
+      <c r="I43" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J43" s="27">
+        <v>0.70065789473684204</v>
+      </c>
+      <c r="K43" s="27">
+        <v>0.9375</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D44" s="27">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="E44" s="27">
+        <v>0.74342105263157898</v>
+      </c>
+      <c r="F44" s="27">
+        <v>0.79276315789473695</v>
+      </c>
+      <c r="G44" s="27">
+        <v>0.875</v>
+      </c>
+      <c r="H44" s="27">
+        <v>0.92434210526315796</v>
+      </c>
+      <c r="I44" s="27">
+        <v>0.53947368421052599</v>
+      </c>
+      <c r="J44" s="27">
+        <v>0.73684210526315796</v>
+      </c>
+      <c r="K44" s="27">
+        <v>0.81907894736842102</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D45" s="27">
+        <v>0.75986842105263197</v>
+      </c>
+      <c r="E45" s="27">
+        <v>0.78947368421052599</v>
+      </c>
+      <c r="F45" s="27">
+        <v>0.72368421052631604</v>
+      </c>
+      <c r="G45" s="27">
+        <v>0.86842105263157898</v>
+      </c>
+      <c r="H45" s="27">
+        <v>0.96710526315789502</v>
+      </c>
+      <c r="I45" s="27">
+        <v>0.53289473684210498</v>
+      </c>
+      <c r="J45" s="27">
+        <v>0.73355263157894701</v>
+      </c>
+      <c r="K45" s="27">
+        <v>0.89802631578947401</v>
+      </c>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D46" s="27">
+        <v>0.90131578947368396</v>
+      </c>
+      <c r="E46" s="27">
+        <v>0.81578947368421095</v>
+      </c>
+      <c r="F46" s="27">
+        <v>0.84868421052631604</v>
+      </c>
+      <c r="G46" s="27">
+        <v>0.88486842105263197</v>
+      </c>
+      <c r="H46" s="27">
+        <v>0.875</v>
+      </c>
+      <c r="I46" s="27">
+        <v>0.90131578947368396</v>
+      </c>
+      <c r="J46" s="27">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="K46" s="27">
+        <v>0.88815789473684204</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D47" s="27">
+        <v>0.87828947368421095</v>
+      </c>
+      <c r="E47" s="27">
+        <v>0.91118421052631604</v>
+      </c>
+      <c r="F47" s="27">
+        <v>0.83552631578947401</v>
+      </c>
+      <c r="G47" s="27">
+        <v>0.95394736842105299</v>
+      </c>
+      <c r="H47" s="27">
+        <v>0.90789473684210498</v>
+      </c>
+      <c r="I47" s="27">
+        <v>0.89802631578947401</v>
+      </c>
+      <c r="J47" s="27">
+        <v>0.75986842105263197</v>
+      </c>
+      <c r="K47" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+    </row>
+    <row r="48" spans="2:11" x14ac:dyDescent="0.3">
+      <c r="D48" s="27">
+        <v>0.51644736842105299</v>
+      </c>
+      <c r="E48" s="27">
+        <v>0.50328947368421095</v>
+      </c>
+      <c r="F48" s="27">
+        <v>0.50657894736842102</v>
+      </c>
+      <c r="G48" s="27">
+        <v>0.50328947368421095</v>
+      </c>
+      <c r="H48" s="27">
+        <v>0.48355263157894701</v>
+      </c>
+      <c r="I48" s="27">
+        <v>0.51315789473684204</v>
+      </c>
+      <c r="J48" s="27">
+        <v>0.51315789473684204</v>
+      </c>
+      <c r="K48" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="49" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D49" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="E49" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="27">
+        <v>0.61513157894736803</v>
+      </c>
+      <c r="G49" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="H49" s="27">
+        <v>0.54934210526315796</v>
+      </c>
+      <c r="I49" s="27">
+        <v>0.52302631578947401</v>
+      </c>
+      <c r="J49" s="27">
+        <v>0.57565789473684204</v>
+      </c>
+      <c r="K49" s="27">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D50" s="27">
+        <v>0.91776315789473695</v>
+      </c>
+      <c r="E50" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="F50" s="27">
+        <v>0.72039473684210498</v>
+      </c>
+      <c r="G50" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="H50" s="27">
+        <v>0.94078947368421095</v>
+      </c>
+      <c r="I50" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J50" s="27">
+        <v>0.77302631578947401</v>
+      </c>
+      <c r="K50" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+    </row>
+    <row r="51" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D51" s="27">
+        <v>0.91776315789473695</v>
+      </c>
+      <c r="E51" s="27">
+        <v>0.90789473684210498</v>
+      </c>
+      <c r="F51" s="27">
+        <v>0.76315789473684204</v>
+      </c>
+      <c r="G51" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="H51" s="27">
+        <v>0.91447368421052599</v>
+      </c>
+      <c r="I51" s="27">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="27">
+        <v>0.63815789473684204</v>
+      </c>
+      <c r="K51" s="27">
+        <v>0.92763157894736803</v>
+      </c>
+    </row>
+    <row r="52" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D52" s="27">
+        <v>0.70394736842105299</v>
+      </c>
+      <c r="E52" s="27">
+        <v>0.71052631578947401</v>
+      </c>
+      <c r="F52" s="27">
+        <v>0.74342105263157898</v>
+      </c>
+      <c r="G52" s="27">
+        <v>0.75986842105263197</v>
+      </c>
+      <c r="H52" s="27">
+        <v>0.82236842105263197</v>
+      </c>
+      <c r="I52" s="27">
+        <v>0.57894736842105299</v>
+      </c>
+      <c r="J52" s="27">
+        <v>0.67763157894736803</v>
+      </c>
+      <c r="K52" s="27">
+        <v>0.72039473684210498</v>
+      </c>
+    </row>
+    <row r="53" spans="4:11" x14ac:dyDescent="0.3">
+      <c r="D53" s="27">
+        <v>0.69078947368421095</v>
+      </c>
+      <c r="E53" s="27">
+        <v>0.73026315789473695</v>
+      </c>
+      <c r="F53" s="27">
+        <v>0.72368421052631604</v>
+      </c>
+      <c r="G53" s="27">
+        <v>0.92763157894736803</v>
+      </c>
+      <c r="H53" s="27">
+        <v>0.92105263157894701</v>
+      </c>
+      <c r="I53" s="27">
+        <v>0.52302631578947401</v>
+      </c>
+      <c r="J53" s="27">
+        <v>0.64473684210526305</v>
+      </c>
+      <c r="K53" s="27">
+        <v>0.875</v>
       </c>
     </row>
   </sheetData>

</xml_diff>